<commit_message>
Reintroduce changes from the region transport modelling
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_CAP21-EAM.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_CAP21-EAM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\TRA_VA5\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21D46DA-BECE-4018-ADD2-14B0CC31CCAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF539782-EBE6-401E-9B3F-4EBB3E48A6A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
   <si>
     <t>LimType</t>
   </si>
@@ -349,9 +349,6 @@
     <t>Pset_PN</t>
   </si>
   <si>
-    <t>T-A*INT*,T-NAV*</t>
-  </si>
-  <si>
     <t>~TFM_INS</t>
   </si>
   <si>
@@ -380,6 +377,9 @@
   </si>
   <si>
     <t>UC_RHSTS</t>
+  </si>
+  <si>
+    <t>T-*</t>
   </si>
 </sst>
 </file>
@@ -387,11 +387,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="???,???.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="???,???.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,8 +495,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8.25"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft Sans Serif"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,8 +559,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F8FF"/>
+        <bgColor rgb="FFF3F8FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -644,10 +661,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" indent="5"/>
@@ -655,13 +687,13 @@
     <xf numFmtId="4" fontId="8" fillId="0" borderId="3" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -671,7 +703,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -682,8 +714,9 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -709,8 +742,12 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="18" fillId="10" borderId="8" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="24">
     <cellStyle name="5x indented GHG Textfiels" xfId="3" xr:uid="{5F614CE9-C529-4323-B893-6D57470EC2CB}"/>
     <cellStyle name="Bold GHG Numbers (0.00)" xfId="4" xr:uid="{68EF4BBB-3F5E-4C7B-A333-BF2B223F0AF2}"/>
     <cellStyle name="Comma 2" xfId="6" xr:uid="{45EC7F75-5971-4A67-99AE-46A786A4824E}"/>
@@ -725,6 +762,7 @@
     <cellStyle name="Normal 6" xfId="12" xr:uid="{D9D2F9CA-BE05-4718-A5D3-63A1935E4B13}"/>
     <cellStyle name="Normal 7" xfId="13" xr:uid="{4A3BD780-B7E2-4620-A3B8-6D7B9E1827CF}"/>
     <cellStyle name="Normal 8" xfId="2" xr:uid="{9CC4C1C2-B822-43DD-AB50-FD4B95F81E3C}"/>
+    <cellStyle name="Normal 9" xfId="23" xr:uid="{C948C00C-F2E9-47A0-9EFC-372956A7D551}"/>
     <cellStyle name="Normal GHG Numbers (0.00)" xfId="14" xr:uid="{4315B456-6133-4E7F-BC4E-BBFBBC638BBD}"/>
     <cellStyle name="Normal GHG whole table" xfId="15" xr:uid="{DF8CE107-6695-4608-ABF3-0494C7C964D1}"/>
     <cellStyle name="Normal GHG-Shade" xfId="16" xr:uid="{BD5DD806-3F9F-4E18-99B5-069CE81720E5}"/>
@@ -770,7 +808,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1162,40 +1200,40 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="1"/>
+    <col min="29" max="29" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -1309,12 +1347,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1429,7 +1467,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1546,7 +1584,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1663,7 +1701,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -1671,7 +1709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -1679,7 +1717,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -1687,7 +1725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
@@ -1695,7 +1733,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
@@ -1703,7 +1741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
@@ -1711,7 +1749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
@@ -1719,7 +1757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
@@ -1727,7 +1765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
@@ -1735,7 +1773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>43</v>
       </c>
@@ -1751,7 +1789,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
@@ -1759,7 +1797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
@@ -1767,7 +1805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
@@ -1775,7 +1813,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>47</v>
       </c>
@@ -1783,7 +1821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
@@ -1791,7 +1829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>49</v>
       </c>
@@ -1799,7 +1837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>50</v>
       </c>
@@ -1807,7 +1845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>51</v>
       </c>
@@ -1815,7 +1853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>52</v>
       </c>
@@ -1823,7 +1861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>53</v>
       </c>
@@ -1831,7 +1869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>54</v>
       </c>
@@ -1839,7 +1877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>55</v>
       </c>
@@ -1847,7 +1885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>56</v>
       </c>
@@ -1855,7 +1893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>57</v>
       </c>
@@ -1863,7 +1901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>58</v>
       </c>
@@ -1871,7 +1909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>59</v>
       </c>
@@ -1879,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>60</v>
       </c>
@@ -1905,7 +1943,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1925,22 +1963,22 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.109375" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.140625" style="8"/>
-    <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="9.109375" style="8"/>
+    <col min="13" max="13" width="10.5546875" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="8"/>
+    <col min="15" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
@@ -1959,7 +1997,7 @@
       <c r="P1"/>
       <c r="Q1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1978,7 +2016,7 @@
       <c r="P2"/>
       <c r="Q2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -1997,7 +2035,7 @@
       <c r="P3"/>
       <c r="Q3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4" t="s">
         <v>61</v>
@@ -2020,7 +2058,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>66</v>
@@ -2043,7 +2081,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>72</v>
       </c>
@@ -2060,40 +2098,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="8">
-        <v>29977</v>
-      </c>
-      <c r="D7" s="8">
-        <v>19600</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="C7" s="21">
+        <v>19527.1004732492</v>
+      </c>
+      <c r="D7" s="21">
+        <v>13415.316698552</v>
+      </c>
+      <c r="E7" s="21">
         <v>0</v>
       </c>
       <c r="F7" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="8" t="str">
-        <f>C8</f>
-        <v>T-A*INT*,T-NAV*</v>
-      </c>
-      <c r="E8" s="8" t="str">
-        <f>D8</f>
-        <v>T-A*INT*,T-NAV*</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>62</v>
       </c>
@@ -2109,7 +2145,7 @@
         <v>*CO2*,-*CO2S</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>71</v>
       </c>
@@ -2125,12 +2161,12 @@
         <v>ENV</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -2146,9 +2182,9 @@
         <v>UP</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="8">
         <v>-1</v>
@@ -2162,10 +2198,10 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -2192,7 +2228,7 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -2211,7 +2247,7 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -2230,7 +2266,7 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -2264,45 +2300,45 @@
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="28.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="8"/>
-    <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="8"/>
+    <col min="2" max="2" width="28.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="8"/>
+    <col min="8" max="8" width="12.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="8"/>
+    <col min="11" max="11" width="27.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -2322,19 +2358,19 @@
         <v>0</v>
       </c>
       <c r="H5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>69</v>
       </c>
@@ -2350,7 +2386,7 @@
       </c>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Single"</f>
         <v>UC_NetZero_CO2_2050_Single</v>
@@ -2377,14 +2413,14 @@
       </c>
       <c r="J7" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)</f>
-        <v>29977</v>
+        <v>19527.1004732492</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>VLOOKUP(K$5, config!$B$4:$F$14,2,FALSE) &amp; " - Single"</f>
         <v>Net Zero CO2 by 2050 - Single</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2395,7 +2431,7 @@
       </c>
       <c r="E8" s="8" t="str">
         <f>VLOOKUP(E$5, config!$B$4:$F$14,2,FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
+        <v>T-*</v>
       </c>
       <c r="F8" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,2,FALSE)</f>
@@ -2406,7 +2442,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2429,10 +2465,10 @@
       </c>
       <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)</f>
-        <v>19600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>13415.316698552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2443,7 +2479,7 @@
       </c>
       <c r="E10" s="8" t="str">
         <f>VLOOKUP(E$5, config!$B$4:$F$14,3,FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
+        <v>T-*</v>
       </c>
       <c r="F10" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,3,FALSE)</f>
@@ -2454,7 +2490,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2480,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C12" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2491,7 +2527,7 @@
       </c>
       <c r="E12" s="8" t="str">
         <f>VLOOKUP(E$5, config!$B$4:$F$14,4,FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
+        <v>T-*</v>
       </c>
       <c r="F12" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,4,FALSE)</f>
@@ -2502,7 +2538,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F13" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,5,FALSE)</f>
         <v>0</v>
@@ -2523,48 +2559,48 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="27.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.109375" style="8"/>
+    <col min="2" max="2" width="27.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -2584,19 +2620,19 @@
         <v>0</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>69</v>
       </c>
@@ -2612,7 +2648,7 @@
       </c>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$F$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_NetZero_CO2_2050_Multi</v>
@@ -2639,14 +2675,14 @@
       </c>
       <c r="J7" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,2,FALSE)</f>
-        <v>29977</v>
+        <v>19527.1004732492</v>
       </c>
       <c r="K7" s="8" t="str">
         <f>VLOOKUP(K$5, config!$B$4:$F$14,2,FALSE) &amp; " - Multi"</f>
         <v>Net Zero CO2 by 2050 - Multi</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C8" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,2,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2657,7 +2693,7 @@
       </c>
       <c r="E8" s="8" t="str">
         <f>VLOOKUP(E$5, config!$B$4:$F$14,2,FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
+        <v>T-*</v>
       </c>
       <c r="F8" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,2,FALSE)</f>
@@ -2668,7 +2704,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2691,10 +2727,10 @@
       </c>
       <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$F$14,3,FALSE)</f>
-        <v>19600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>13415.316698552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,3,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2705,7 +2741,7 @@
       </c>
       <c r="E10" s="8" t="str">
         <f>VLOOKUP(E$5, config!$B$4:$F$14,3,FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
+        <v>T-*</v>
       </c>
       <c r="F10" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,3,FALSE)</f>
@@ -2716,7 +2752,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C11" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2742,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C12" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$F$14,4,FALSE)</f>
         <v>*CO2*,-*CO2S</v>
@@ -2753,7 +2789,7 @@
       </c>
       <c r="E12" s="8" t="str">
         <f>VLOOKUP(E$5, config!$B$4:$F$14,4,FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
+        <v>T-*</v>
       </c>
       <c r="F12" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,4,FALSE)</f>
@@ -2764,7 +2800,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F13" s="8">
         <f>VLOOKUP(F$5, config!$B$4:$F$14,5,FALSE)</f>
         <v>0</v>
@@ -2788,17 +2824,17 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -2807,15 +2843,15 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>72</v>
@@ -2832,19 +2868,19 @@
         <v>National</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
       <c r="C4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" s="19">
         <v>-1</v>

</xml_diff>